<commit_message>
email data working with email donation upload with donation
</commit_message>
<xml_diff>
--- a/D:\test excel\EmailComparisonReport-17647483501.xlsx
+++ b/D:\test excel\EmailComparisonReport-17647483501.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E4131ED5-B661-004E-B50C-B283CA9DD0F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D9DCFAEA-566A-7C49-BD00-5ABF272C9596}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="500" windowWidth="25440" windowHeight="14260"/>
   </bookViews>
@@ -49,22 +49,22 @@
     <t xml:space="preserve">Unique Opens </t>
   </si>
   <si>
-    <t>2.25.21.EOM2</t>
-  </si>
-  <si>
     <t>run4off + 60dayopeners + 30 day new subs</t>
   </si>
   <si>
     <t>Press-all (For suppression)</t>
   </si>
   <si>
-    <t>TestEmail</t>
-  </si>
-  <si>
     <t>Refcode</t>
   </si>
   <si>
     <t>2021-02-25 04:51:35</t>
+  </si>
+  <si>
+    <t>tester23</t>
+  </si>
+  <si>
+    <t>3.25.21.EOM2</t>
   </si>
 </sst>
 </file>
@@ -909,7 +909,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -947,24 +947,24 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>38091</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>378</v>
@@ -979,7 +979,7 @@
         <v>8333</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>